<commit_message>
Tiered up Alts and Ancient Shards. Re-added talismans. Added Imbued Wand to highlihgting. Toggled off Chaos Recipe. Thanks to twitch.tv/ArphenLive <3
</commit_message>
<xml_diff>
--- a/Scraps.xlsx
+++ b/Scraps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7005BB1-B25B-46C2-853A-EB4FCB6378CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD75852-F868-4589-97B5-244E990801B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
     <tableColumn id="11" xr3:uid="{95F7E819-E647-494C-8238-F481831E69C0}" name="Pink" dataDxfId="1"/>
     <tableColumn id="12" xr3:uid="{0FCFA7DE-2A3F-4E03-8A66-5509406562C9}" name="Purple" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleDark8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleDark8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DA35C1-A445-4EB5-A4F2-B7757F825CF9}">
   <dimension ref="B2:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Primary update for Expedition. Items not tiered. Additional updates to follow
</commit_message>
<xml_diff>
--- a/Scraps.xlsx
+++ b/Scraps.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD75852-F868-4589-97B5-244E990801B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAFEC4F-8357-4013-8673-BA92DC5C1CC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Icons" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="111">
   <si>
     <t>Circle</t>
   </si>
@@ -363,6 +364,9 @@
   </si>
   <si>
     <t>Divine Vessel</t>
+  </si>
+  <si>
+    <t>High Tier Uniques</t>
   </si>
 </sst>
 </file>
@@ -789,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DA35C1-A445-4EB5-A4F2-B7757F825CF9}">
   <dimension ref="B2:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,7 +1333,9 @@
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
@@ -1496,4 +1502,16 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45DE49A-AA66-4389-9BB9-2C2AF6D898BA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Complete rework of the Minimap icons for all items
</commit_message>
<xml_diff>
--- a/Scraps.xlsx
+++ b/Scraps.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAFEC4F-8357-4013-8673-BA92DC5C1CC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300F25D0-8A78-420E-A2F4-C1F812D05BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
+    <workbookView minimized="1" xWindow="18885" yWindow="1485" windowWidth="19065" windowHeight="14805" activeTab="1" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Icons" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Icons 2024 Rework" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +34,1340 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="132">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="14"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="15"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="16"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="17"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="18"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="19"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="20"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="21"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="22"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="23"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="24"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="25"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="26"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="27"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="28"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="29"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="30"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="31"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="32"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="33"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="34"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="35"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="36"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="37"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="38"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="39"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="40"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="41"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="42"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="43"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="44"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="45"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="46"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="47"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="48"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="49"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="50"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="51"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="52"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="53"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="54"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="55"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="56"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="57"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="58"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="59"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="60"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="61"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="62"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="63"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="64"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="65"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="66"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="67"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="68"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="69"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="70"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="71"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="72"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="73"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="74"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="75"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="76"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="77"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="78"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="79"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="80"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="81"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="82"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="83"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="84"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="85"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="86"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="87"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="88"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="89"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="90"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="91"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="92"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="93"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="94"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="95"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="96"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="97"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="98"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="99"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="100"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="101"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="102"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="103"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="104"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="105"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="106"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="107"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="108"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="109"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="110"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="111"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="112"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="113"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="114"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="115"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="116"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="117"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="118"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="119"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="120"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="121"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="122"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="123"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="124"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="125"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="126"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="127"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="128"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="129"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="130"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="131"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="132">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
+    <bk>
+      <rc t="1" v="14"/>
+    </bk>
+    <bk>
+      <rc t="1" v="15"/>
+    </bk>
+    <bk>
+      <rc t="1" v="16"/>
+    </bk>
+    <bk>
+      <rc t="1" v="17"/>
+    </bk>
+    <bk>
+      <rc t="1" v="18"/>
+    </bk>
+    <bk>
+      <rc t="1" v="19"/>
+    </bk>
+    <bk>
+      <rc t="1" v="20"/>
+    </bk>
+    <bk>
+      <rc t="1" v="21"/>
+    </bk>
+    <bk>
+      <rc t="1" v="22"/>
+    </bk>
+    <bk>
+      <rc t="1" v="23"/>
+    </bk>
+    <bk>
+      <rc t="1" v="24"/>
+    </bk>
+    <bk>
+      <rc t="1" v="25"/>
+    </bk>
+    <bk>
+      <rc t="1" v="26"/>
+    </bk>
+    <bk>
+      <rc t="1" v="27"/>
+    </bk>
+    <bk>
+      <rc t="1" v="28"/>
+    </bk>
+    <bk>
+      <rc t="1" v="29"/>
+    </bk>
+    <bk>
+      <rc t="1" v="30"/>
+    </bk>
+    <bk>
+      <rc t="1" v="31"/>
+    </bk>
+    <bk>
+      <rc t="1" v="32"/>
+    </bk>
+    <bk>
+      <rc t="1" v="33"/>
+    </bk>
+    <bk>
+      <rc t="1" v="34"/>
+    </bk>
+    <bk>
+      <rc t="1" v="35"/>
+    </bk>
+    <bk>
+      <rc t="1" v="36"/>
+    </bk>
+    <bk>
+      <rc t="1" v="37"/>
+    </bk>
+    <bk>
+      <rc t="1" v="38"/>
+    </bk>
+    <bk>
+      <rc t="1" v="39"/>
+    </bk>
+    <bk>
+      <rc t="1" v="40"/>
+    </bk>
+    <bk>
+      <rc t="1" v="41"/>
+    </bk>
+    <bk>
+      <rc t="1" v="42"/>
+    </bk>
+    <bk>
+      <rc t="1" v="43"/>
+    </bk>
+    <bk>
+      <rc t="1" v="44"/>
+    </bk>
+    <bk>
+      <rc t="1" v="45"/>
+    </bk>
+    <bk>
+      <rc t="1" v="46"/>
+    </bk>
+    <bk>
+      <rc t="1" v="47"/>
+    </bk>
+    <bk>
+      <rc t="1" v="48"/>
+    </bk>
+    <bk>
+      <rc t="1" v="49"/>
+    </bk>
+    <bk>
+      <rc t="1" v="50"/>
+    </bk>
+    <bk>
+      <rc t="1" v="51"/>
+    </bk>
+    <bk>
+      <rc t="1" v="52"/>
+    </bk>
+    <bk>
+      <rc t="1" v="53"/>
+    </bk>
+    <bk>
+      <rc t="1" v="54"/>
+    </bk>
+    <bk>
+      <rc t="1" v="55"/>
+    </bk>
+    <bk>
+      <rc t="1" v="56"/>
+    </bk>
+    <bk>
+      <rc t="1" v="57"/>
+    </bk>
+    <bk>
+      <rc t="1" v="58"/>
+    </bk>
+    <bk>
+      <rc t="1" v="59"/>
+    </bk>
+    <bk>
+      <rc t="1" v="60"/>
+    </bk>
+    <bk>
+      <rc t="1" v="61"/>
+    </bk>
+    <bk>
+      <rc t="1" v="62"/>
+    </bk>
+    <bk>
+      <rc t="1" v="63"/>
+    </bk>
+    <bk>
+      <rc t="1" v="64"/>
+    </bk>
+    <bk>
+      <rc t="1" v="65"/>
+    </bk>
+    <bk>
+      <rc t="1" v="66"/>
+    </bk>
+    <bk>
+      <rc t="1" v="67"/>
+    </bk>
+    <bk>
+      <rc t="1" v="68"/>
+    </bk>
+    <bk>
+      <rc t="1" v="69"/>
+    </bk>
+    <bk>
+      <rc t="1" v="70"/>
+    </bk>
+    <bk>
+      <rc t="1" v="71"/>
+    </bk>
+    <bk>
+      <rc t="1" v="72"/>
+    </bk>
+    <bk>
+      <rc t="1" v="73"/>
+    </bk>
+    <bk>
+      <rc t="1" v="74"/>
+    </bk>
+    <bk>
+      <rc t="1" v="75"/>
+    </bk>
+    <bk>
+      <rc t="1" v="76"/>
+    </bk>
+    <bk>
+      <rc t="1" v="77"/>
+    </bk>
+    <bk>
+      <rc t="1" v="78"/>
+    </bk>
+    <bk>
+      <rc t="1" v="79"/>
+    </bk>
+    <bk>
+      <rc t="1" v="80"/>
+    </bk>
+    <bk>
+      <rc t="1" v="81"/>
+    </bk>
+    <bk>
+      <rc t="1" v="82"/>
+    </bk>
+    <bk>
+      <rc t="1" v="83"/>
+    </bk>
+    <bk>
+      <rc t="1" v="84"/>
+    </bk>
+    <bk>
+      <rc t="1" v="85"/>
+    </bk>
+    <bk>
+      <rc t="1" v="86"/>
+    </bk>
+    <bk>
+      <rc t="1" v="87"/>
+    </bk>
+    <bk>
+      <rc t="1" v="88"/>
+    </bk>
+    <bk>
+      <rc t="1" v="89"/>
+    </bk>
+    <bk>
+      <rc t="1" v="90"/>
+    </bk>
+    <bk>
+      <rc t="1" v="91"/>
+    </bk>
+    <bk>
+      <rc t="1" v="92"/>
+    </bk>
+    <bk>
+      <rc t="1" v="93"/>
+    </bk>
+    <bk>
+      <rc t="1" v="94"/>
+    </bk>
+    <bk>
+      <rc t="1" v="95"/>
+    </bk>
+    <bk>
+      <rc t="1" v="96"/>
+    </bk>
+    <bk>
+      <rc t="1" v="97"/>
+    </bk>
+    <bk>
+      <rc t="1" v="98"/>
+    </bk>
+    <bk>
+      <rc t="1" v="99"/>
+    </bk>
+    <bk>
+      <rc t="1" v="100"/>
+    </bk>
+    <bk>
+      <rc t="1" v="101"/>
+    </bk>
+    <bk>
+      <rc t="1" v="102"/>
+    </bk>
+    <bk>
+      <rc t="1" v="103"/>
+    </bk>
+    <bk>
+      <rc t="1" v="104"/>
+    </bk>
+    <bk>
+      <rc t="1" v="105"/>
+    </bk>
+    <bk>
+      <rc t="1" v="106"/>
+    </bk>
+    <bk>
+      <rc t="1" v="107"/>
+    </bk>
+    <bk>
+      <rc t="1" v="108"/>
+    </bk>
+    <bk>
+      <rc t="1" v="109"/>
+    </bk>
+    <bk>
+      <rc t="1" v="110"/>
+    </bk>
+    <bk>
+      <rc t="1" v="111"/>
+    </bk>
+    <bk>
+      <rc t="1" v="112"/>
+    </bk>
+    <bk>
+      <rc t="1" v="113"/>
+    </bk>
+    <bk>
+      <rc t="1" v="114"/>
+    </bk>
+    <bk>
+      <rc t="1" v="115"/>
+    </bk>
+    <bk>
+      <rc t="1" v="116"/>
+    </bk>
+    <bk>
+      <rc t="1" v="117"/>
+    </bk>
+    <bk>
+      <rc t="1" v="118"/>
+    </bk>
+    <bk>
+      <rc t="1" v="119"/>
+    </bk>
+    <bk>
+      <rc t="1" v="120"/>
+    </bk>
+    <bk>
+      <rc t="1" v="121"/>
+    </bk>
+    <bk>
+      <rc t="1" v="122"/>
+    </bk>
+    <bk>
+      <rc t="1" v="123"/>
+    </bk>
+    <bk>
+      <rc t="1" v="124"/>
+    </bk>
+    <bk>
+      <rc t="1" v="125"/>
+    </bk>
+    <bk>
+      <rc t="1" v="126"/>
+    </bk>
+    <bk>
+      <rc t="1" v="127"/>
+    </bk>
+    <bk>
+      <rc t="1" v="128"/>
+    </bk>
+    <bk>
+      <rc t="1" v="129"/>
+    </bk>
+    <bk>
+      <rc t="1" v="130"/>
+    </bk>
+    <bk>
+      <rc t="1" v="131"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="200">
   <si>
     <t>Circle</t>
   </si>
@@ -367,6 +1700,273 @@
   </si>
   <si>
     <t>High Tier Uniques</t>
+  </si>
+  <si>
+    <t>UpsideDownHouse</t>
+  </si>
+  <si>
+    <t>Maps</t>
+  </si>
+  <si>
+    <t>Splinters</t>
+  </si>
+  <si>
+    <t>Div Cards</t>
+  </si>
+  <si>
+    <t>Catalysts</t>
+  </si>
+  <si>
+    <t>Basic Currency</t>
+  </si>
+  <si>
+    <t>High Tier</t>
+  </si>
+  <si>
+    <t>Veiled Items</t>
+  </si>
+  <si>
+    <t>Delirium Orbs</t>
+  </si>
+  <si>
+    <t>Legion Splinters/Incubators</t>
+  </si>
+  <si>
+    <t>Tier 16</t>
+  </si>
+  <si>
+    <t>Unique Map</t>
+  </si>
+  <si>
+    <t>Heist Contract</t>
+  </si>
+  <si>
+    <t>Heist Blueprint</t>
+  </si>
+  <si>
+    <t>T1-5 Map</t>
+  </si>
+  <si>
+    <t>T6-10 Map</t>
+  </si>
+  <si>
+    <t>T11-15 Map</t>
+  </si>
+  <si>
+    <t>Valdo's/Voidborn</t>
+  </si>
+  <si>
+    <t>Rogue's Markers</t>
+  </si>
+  <si>
+    <t>Logbooks</t>
+  </si>
+  <si>
+    <t>Blight Map</t>
+  </si>
+  <si>
+    <t>Guardian Map</t>
+  </si>
+  <si>
+    <t>Sim Splinters</t>
+  </si>
+  <si>
+    <t>Crescent</t>
+  </si>
+  <si>
+    <t>Ritual Splinters</t>
+  </si>
+  <si>
+    <t>Breach Splinters</t>
+  </si>
+  <si>
+    <t>Legion Splinters</t>
+  </si>
+  <si>
+    <t>Chaos</t>
+  </si>
+  <si>
+    <t>Divine</t>
+  </si>
+  <si>
+    <t>Vaal Orb</t>
+  </si>
+  <si>
+    <t>Sextant</t>
+  </si>
+  <si>
+    <t>Eldritch</t>
+  </si>
+  <si>
+    <t>Instilling/Enkindling</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>Vivid</t>
+  </si>
+  <si>
+    <t>Wild</t>
+  </si>
+  <si>
+    <t>Primal</t>
+  </si>
+  <si>
+    <t>Sac Frag</t>
+  </si>
+  <si>
+    <t>Mortal Frag</t>
+  </si>
+  <si>
+    <t>Elder</t>
+  </si>
+  <si>
+    <t>Shaper</t>
+  </si>
+  <si>
+    <t>Scarab</t>
+  </si>
+  <si>
+    <t>Winged</t>
+  </si>
+  <si>
+    <t>Gilded</t>
+  </si>
+  <si>
+    <t>Rusted</t>
+  </si>
+  <si>
+    <t>Polished</t>
+  </si>
+  <si>
+    <t>Uber Elder</t>
+  </si>
+  <si>
+    <t>Non T0</t>
+  </si>
+  <si>
+    <t>Vaal Gems</t>
+  </si>
+  <si>
+    <t>Gems</t>
+  </si>
+  <si>
+    <t>Awakened</t>
+  </si>
+  <si>
+    <t>Trans Gems</t>
+  </si>
+  <si>
+    <t>Level 21/23 Qual</t>
+  </si>
+  <si>
+    <t>Maven's Invitation</t>
+  </si>
+  <si>
+    <t>Atlas Invitation</t>
+  </si>
+  <si>
+    <t>Eldritch Invitation</t>
+  </si>
+  <si>
+    <t>Legion Emblem</t>
+  </si>
+  <si>
+    <t>Eye Jewels</t>
+  </si>
+  <si>
+    <t>League Rewards</t>
+  </si>
+  <si>
+    <t>Exped Reroll</t>
+  </si>
+  <si>
+    <t>Incubators</t>
+  </si>
+  <si>
+    <t>Offering</t>
+  </si>
+  <si>
+    <t>Lifeforce/Oil</t>
+  </si>
+  <si>
+    <t>Sacred Blossom</t>
+  </si>
+  <si>
+    <t>Golden Oil</t>
+  </si>
+  <si>
+    <t>Shaper/Elder</t>
+  </si>
+  <si>
+    <t>Elderslayer</t>
+  </si>
+  <si>
+    <t>Affliction Charms/Tinctures</t>
+  </si>
+  <si>
+    <t>Cluster Jewels</t>
+  </si>
+  <si>
+    <t>Influenced Item</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>Redeemer</t>
+  </si>
+  <si>
+    <t>Warlord</t>
+  </si>
+  <si>
+    <t>Crusader</t>
+  </si>
+  <si>
+    <t>Fractured</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Heist Base</t>
+  </si>
+  <si>
+    <t>Synthesised</t>
+  </si>
+  <si>
+    <t>Double Corrupted</t>
+  </si>
+  <si>
+    <t>Atlas Bases</t>
+  </si>
+  <si>
+    <t>Tainted Currency</t>
+  </si>
+  <si>
+    <t>Exalt/Veiled</t>
+  </si>
+  <si>
+    <t>Chisel/Regret/Scour</t>
+  </si>
+  <si>
+    <t>Alteration/Horizons</t>
+  </si>
+  <si>
+    <t>Stacked Decks</t>
+  </si>
+  <si>
+    <t>Exceptional</t>
+  </si>
+  <si>
+    <t>6 Linked</t>
   </si>
 </sst>
 </file>
@@ -390,7 +1990,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -398,11 +1998,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -411,6 +2040,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -471,6 +2124,725 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="132">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>7</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>8</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>14</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>15</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>16</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>17</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>18</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>19</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>20</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>21</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>22</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>23</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>24</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>25</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>26</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>27</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>28</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>29</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>30</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>31</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>32</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>33</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>34</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>35</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>36</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>37</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>38</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>39</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>40</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>41</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>42</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>43</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>44</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>45</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>46</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>47</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>48</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>49</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>50</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>51</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>52</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>53</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>54</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>55</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>56</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>57</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>58</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>59</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>60</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>61</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>62</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>63</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>64</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>65</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>66</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>67</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>68</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>69</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>70</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>71</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>72</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>73</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>74</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>75</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>76</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>77</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>78</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>79</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>80</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>81</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>82</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>83</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>84</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>85</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>86</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>87</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>88</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>89</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>90</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>91</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>92</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>93</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>94</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>95</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>96</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>97</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>98</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>99</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>100</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>101</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>102</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>103</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>104</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>105</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>106</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>107</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>108</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>109</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>110</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>111</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>112</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>113</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>114</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>115</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>116</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>117</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>118</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>119</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>120</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>121</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>122</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>123</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>124</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>125</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>126</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>127</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>128</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>129</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>130</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>131</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+  <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
+  <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
+  <rel r:id="rId15"/>
+  <rel r:id="rId16"/>
+  <rel r:id="rId17"/>
+  <rel r:id="rId18"/>
+  <rel r:id="rId19"/>
+  <rel r:id="rId20"/>
+  <rel r:id="rId21"/>
+  <rel r:id="rId22"/>
+  <rel r:id="rId23"/>
+  <rel r:id="rId24"/>
+  <rel r:id="rId25"/>
+  <rel r:id="rId26"/>
+  <rel r:id="rId27"/>
+  <rel r:id="rId28"/>
+  <rel r:id="rId29"/>
+  <rel r:id="rId30"/>
+  <rel r:id="rId31"/>
+  <rel r:id="rId32"/>
+  <rel r:id="rId33"/>
+  <rel r:id="rId34"/>
+  <rel r:id="rId35"/>
+  <rel r:id="rId36"/>
+  <rel r:id="rId37"/>
+  <rel r:id="rId38"/>
+  <rel r:id="rId39"/>
+  <rel r:id="rId40"/>
+  <rel r:id="rId41"/>
+  <rel r:id="rId42"/>
+  <rel r:id="rId43"/>
+  <rel r:id="rId44"/>
+  <rel r:id="rId45"/>
+  <rel r:id="rId46"/>
+  <rel r:id="rId47"/>
+  <rel r:id="rId48"/>
+  <rel r:id="rId49"/>
+  <rel r:id="rId50"/>
+  <rel r:id="rId51"/>
+  <rel r:id="rId52"/>
+  <rel r:id="rId53"/>
+  <rel r:id="rId54"/>
+  <rel r:id="rId55"/>
+  <rel r:id="rId56"/>
+  <rel r:id="rId57"/>
+  <rel r:id="rId58"/>
+  <rel r:id="rId59"/>
+  <rel r:id="rId60"/>
+  <rel r:id="rId61"/>
+  <rel r:id="rId62"/>
+  <rel r:id="rId63"/>
+  <rel r:id="rId64"/>
+  <rel r:id="rId65"/>
+  <rel r:id="rId66"/>
+  <rel r:id="rId67"/>
+  <rel r:id="rId68"/>
+  <rel r:id="rId69"/>
+  <rel r:id="rId70"/>
+  <rel r:id="rId71"/>
+  <rel r:id="rId72"/>
+  <rel r:id="rId73"/>
+  <rel r:id="rId74"/>
+  <rel r:id="rId75"/>
+  <rel r:id="rId76"/>
+  <rel r:id="rId77"/>
+  <rel r:id="rId78"/>
+  <rel r:id="rId79"/>
+  <rel r:id="rId80"/>
+  <rel r:id="rId81"/>
+  <rel r:id="rId82"/>
+  <rel r:id="rId83"/>
+  <rel r:id="rId84"/>
+  <rel r:id="rId85"/>
+  <rel r:id="rId86"/>
+  <rel r:id="rId87"/>
+  <rel r:id="rId88"/>
+  <rel r:id="rId89"/>
+  <rel r:id="rId90"/>
+  <rel r:id="rId91"/>
+  <rel r:id="rId92"/>
+  <rel r:id="rId93"/>
+  <rel r:id="rId94"/>
+  <rel r:id="rId95"/>
+  <rel r:id="rId96"/>
+  <rel r:id="rId97"/>
+  <rel r:id="rId98"/>
+  <rel r:id="rId99"/>
+  <rel r:id="rId100"/>
+  <rel r:id="rId101"/>
+  <rel r:id="rId102"/>
+  <rel r:id="rId103"/>
+  <rel r:id="rId104"/>
+  <rel r:id="rId105"/>
+  <rel r:id="rId106"/>
+  <rel r:id="rId107"/>
+  <rel r:id="rId108"/>
+  <rel r:id="rId109"/>
+  <rel r:id="rId110"/>
+  <rel r:id="rId111"/>
+  <rel r:id="rId112"/>
+  <rel r:id="rId113"/>
+  <rel r:id="rId114"/>
+  <rel r:id="rId115"/>
+  <rel r:id="rId116"/>
+  <rel r:id="rId117"/>
+  <rel r:id="rId118"/>
+  <rel r:id="rId119"/>
+  <rel r:id="rId120"/>
+  <rel r:id="rId121"/>
+  <rel r:id="rId122"/>
+  <rel r:id="rId123"/>
+  <rel r:id="rId124"/>
+  <rel r:id="rId125"/>
+  <rel r:id="rId126"/>
+  <rel r:id="rId127"/>
+  <rel r:id="rId128"/>
+  <rel r:id="rId129"/>
+  <rel r:id="rId130"/>
+  <rel r:id="rId131"/>
+  <rel r:id="rId132"/>
+</richValueRels>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -793,8 +3165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DA35C1-A445-4EB5-A4F2-B7757F825CF9}">
   <dimension ref="B2:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,6 +3877,1280 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EF3207-198A-49F7-97F5-E86C821AC6FF}">
+  <dimension ref="A1:Y27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X14" sqref="A1:X14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="5" style="1" customWidth="1"/>
+    <col min="24" max="24" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="3"/>
+    </row>
+    <row r="2" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="11" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="10" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="10" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="I3" s="10" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="K3" s="10" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="M3" s="10" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="O3" s="10" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q3" s="10" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="S3" s="10" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="U3" s="10" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="W3" s="10" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y3" s="3"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="8" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="3" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I4" s="3" t="e" vm="15">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3" t="e" vm="16">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M4" s="3" t="e" vm="17">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="O4" s="3" t="e" vm="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q4" s="3" t="e" vm="19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3" t="e" vm="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="U4" s="3" t="e" vm="21">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3" t="e" vm="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="8" t="e" vm="23">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="3" t="e" vm="24">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G5" s="3" t="e" vm="25">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I5" s="3" t="e" vm="26">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3" t="e" vm="27">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="3" t="e" vm="28">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O5" s="3" t="e" vm="29">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q5" s="3" t="e" vm="30">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="S5" s="3" t="e" vm="31">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3" t="e" vm="32">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="W5" s="3" t="e" vm="33">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y5" s="3"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="8" t="e" vm="34">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="3" t="e" vm="35">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" s="3" t="e" vm="36">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="3" t="e" vm="37">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="3" t="e" vm="38">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M6" s="3" t="e" vm="39">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="O6" s="3" t="e" vm="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q6" s="3" t="e" vm="41">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="S6" s="3" t="e" vm="42">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="U6" s="3" t="e" vm="43">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="W6" s="3" t="e" vm="44">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y6" s="3"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="8" t="e" vm="45">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" s="3" t="e" vm="46">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="e" vm="47">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="e" vm="48">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K7" s="3" t="e" vm="49">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="e" vm="50">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="O7" s="3" t="e" vm="51">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q7" s="3" t="e" vm="52">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="S7" s="3" t="e" vm="53">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="U7" s="3" t="e" vm="54">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3" t="e" vm="55">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="8" t="e" vm="56">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="3" t="e" vm="57">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="e" vm="58">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I8" s="3" t="e" vm="59">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3" t="e" vm="60">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M8" s="3" t="e" vm="61">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O8" s="3" t="e" vm="62">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q8" s="3" t="e" vm="63">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3" t="e" vm="64">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="U8" s="3" t="e" vm="65">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3" t="e" vm="66">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="8" t="e" vm="67">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="3" t="e" vm="68">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="e" vm="69">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="3" t="e" vm="70">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K9" s="3" t="e" vm="71">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="M9" s="3" t="e" vm="72">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="3" t="e" vm="73">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3" t="e" vm="74">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3" t="e" vm="75">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="U9" s="3" t="e" vm="76">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3" t="e" vm="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="8" t="e" vm="78">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E10" s="3" t="e" vm="79">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G10" s="3" t="e" vm="80">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3" t="e" vm="81">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3" t="e" vm="82">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3" t="e" vm="83">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="O10" s="3" t="e" vm="84">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q10" s="3" t="e" vm="85">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="S10" s="3" t="e" vm="86">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3" t="e" vm="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3" t="e" vm="88">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y10" s="3"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="8" t="e" vm="89">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="3" t="e" vm="90">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="3" t="e" vm="91">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="e" vm="92">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K11" s="3" t="e" vm="93">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="M11" s="3" t="e" vm="94">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O11" s="3" t="e" vm="95">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q11" s="3" t="e" vm="96">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3" t="e" vm="97">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="U11" s="3" t="e" vm="98">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3" t="e" vm="99">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y11" s="3"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="8" t="e" vm="100">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="3" t="e" vm="101">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="e" vm="102">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3" t="e" vm="103">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3" t="e" vm="104">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3" t="e" vm="105">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3" t="e" vm="106">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3" t="e" vm="107">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="S12" s="3" t="e" vm="108">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="U12" s="3" t="e" vm="109">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="W12" s="3" t="e" vm="110">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y12" s="3"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="8" t="e" vm="111">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" s="3" t="e" vm="112">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" s="3" t="e" vm="113">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="3" t="e" vm="114">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="K13" s="3" t="e" vm="115">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="M13" s="3" t="e" vm="116">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="O13" s="3" t="e" vm="117">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q13" s="3" t="e" vm="118">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="S13" s="3" t="e" vm="119">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="U13" s="3" t="e" vm="120">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="W13" s="3" t="e" vm="121">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y13" s="3"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="8" t="e" vm="122">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="3" t="e" vm="123">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="e" vm="124">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="I14" s="3" t="e" vm="125">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3" t="e" vm="126">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3" t="e" vm="127">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3" t="e" vm="128">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q14" s="3" t="e" vm="129">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="S14" s="3" t="e" vm="130">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="U14" s="3" t="e" vm="131">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3" t="e" vm="132">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="3"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="3"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="3"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="3"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="3"/>
+    </row>
+    <row r="27" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45DE49A-AA66-4389-9BB9-2C2AF6D898BA}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Rework of filter conversion script to replace alert sounds with native sounds.
</commit_message>
<xml_diff>
--- a/Scraps.xlsx
+++ b/Scraps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300F25D0-8A78-420E-A2F4-C1F812D05BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E257C0-EB57-45FA-B9FC-1A456566C57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="18885" yWindow="1485" windowWidth="19065" windowHeight="14805" activeTab="1" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Icons" sheetId="1" r:id="rId1"/>
@@ -1367,7 +1367,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="200">
   <si>
     <t>Circle</t>
   </si>
@@ -1729,9 +1729,6 @@
     <t>Delirium Orbs</t>
   </si>
   <si>
-    <t>Legion Splinters/Incubators</t>
-  </si>
-  <si>
     <t>Tier 16</t>
   </si>
   <si>
@@ -1759,9 +1756,6 @@
     <t>Rogue's Markers</t>
   </si>
   <si>
-    <t>Logbooks</t>
-  </si>
-  <si>
     <t>Blight Map</t>
   </si>
   <si>
@@ -1967,6 +1961,12 @@
   </si>
   <si>
     <t>6 Linked</t>
+  </si>
+  <si>
+    <t>Logbooks/Memory</t>
+  </si>
+  <si>
+    <t>Unique</t>
   </si>
 </sst>
 </file>
@@ -2031,7 +2031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2045,25 +2045,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3166,7 +3160,7 @@
   <dimension ref="B2:N29"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:L25"/>
+      <selection activeCell="M29" sqref="B17:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,7 +3875,7 @@
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="X14" sqref="A1:X14"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3901,7 +3895,7 @@
     <col min="13" max="13" width="5" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.28515625" style="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5" style="1" customWidth="1"/>
     <col min="18" max="18" width="14.28515625" style="1" customWidth="1"/>
     <col min="19" max="19" width="5" style="1" customWidth="1"/>
@@ -3915,57 +3909,57 @@
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5" t="s">
+      <c r="N1" s="8"/>
+      <c r="O1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5" t="s">
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5" t="s">
+      <c r="R1" s="8"/>
+      <c r="S1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5" t="s">
+      <c r="T1" s="8"/>
+      <c r="U1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5" t="s">
+      <c r="V1" s="8"/>
+      <c r="W1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="5"/>
+      <c r="X1" s="8"/>
       <c r="Y1" s="3"/>
     </row>
     <row r="2" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -3993,77 +3987,77 @@
       <c r="Y2" s="3"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="11" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="7" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="6" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="6" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="I3" s="6" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="K3" s="6" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="M3" s="6" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="O3" s="6" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="10" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="G3" s="10" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="I3" s="10" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="K3" s="10" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="M3" s="10" t="e" vm="6">
-        <v>#VALUE!</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="O3" s="10" t="e" vm="7">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q3" s="10" t="e" vm="8">
-        <v>#VALUE!</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="S3" s="10" t="e" vm="9">
-        <v>#VALUE!</v>
-      </c>
-      <c r="T3" s="10" t="s">
+      <c r="Q3" s="6" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="U3" s="10" t="e" vm="10">
-        <v>#VALUE!</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="W3" s="10" t="e" vm="11">
+      <c r="S3" s="6" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="U3" s="6" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="W3" s="6" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Y3" s="3"/>
     </row>
@@ -4072,12 +4066,12 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" s="8" t="e" vm="12">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D4" s="9"/>
+        <v>152</v>
+      </c>
+      <c r="C4" s="5" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="3" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
@@ -4093,19 +4087,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="M4" s="3" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O4" s="3" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Q4" s="3" t="e" vm="19">
         <v>#VALUE!</v>
@@ -4115,7 +4109,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="U4" s="3" t="e" vm="21">
         <v>#VALUE!</v>
@@ -4132,25 +4126,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C5" s="8" t="e" vm="23">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D5" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="5" t="e" vm="23">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>115</v>
       </c>
       <c r="E5" s="3" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="3" t="e" vm="25">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="G5" s="3" t="e" vm="25">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="I5" s="3" t="e" vm="26">
         <v>#VALUE!</v>
@@ -4185,13 +4179,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="W5" s="3" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Y5" s="3"/>
     </row>
@@ -4202,71 +4196,71 @@
       <c r="B6" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="8" t="e" vm="34">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="5" t="e" vm="34">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="3" t="e" vm="35">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="3" t="e" vm="36">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="3" t="e" vm="37">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K6" s="3" t="e" vm="38">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="3" t="e" vm="39">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="O6" s="3" t="e" vm="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q6" s="3" t="e" vm="41">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="S6" s="3" t="e" vm="42">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T6" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E6" s="3" t="e" vm="35">
-        <v>#VALUE!</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6" s="3" t="e" vm="36">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="I6" s="3" t="e" vm="37">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="U6" s="3" t="e" vm="43">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V6" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="K6" s="3" t="e" vm="38">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="M6" s="3" t="e" vm="39">
-        <v>#VALUE!</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="O6" s="3" t="e" vm="40">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q6" s="3" t="e" vm="41">
-        <v>#VALUE!</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="S6" s="3" t="e" vm="42">
-        <v>#VALUE!</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="U6" s="3" t="e" vm="43">
-        <v>#VALUE!</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="W6" s="3" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y6" s="3"/>
     </row>
@@ -4275,13 +4269,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C7" s="8" t="e" vm="45">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
+      </c>
+      <c r="C7" s="5" t="e" vm="45">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E7" s="3" t="e" vm="46">
         <v>#VALUE!</v>
@@ -4295,7 +4289,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K7" s="3" t="e" vm="49">
         <v>#VALUE!</v>
@@ -4305,25 +4299,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="O7" s="3" t="e" vm="51">
         <v>#VALUE!</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q7" s="3" t="e" vm="52">
         <v>#VALUE!</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="S7" s="3" t="e" vm="53">
         <v>#VALUE!</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="U7" s="3" t="e" vm="54">
         <v>#VALUE!</v>
@@ -4340,13 +4334,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C8" s="8" t="e" vm="56">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>191</v>
+        <v>186</v>
+      </c>
+      <c r="C8" s="5" t="e" vm="56">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="E8" s="3" t="e" vm="57">
         <v>#VALUE!</v>
@@ -4356,7 +4350,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I8" s="3" t="e" vm="59">
         <v>#VALUE!</v>
@@ -4366,7 +4360,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M8" s="3" t="e" vm="61">
         <v>#VALUE!</v>
@@ -4378,7 +4372,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="Q8" s="3" t="e" vm="63">
         <v>#VALUE!</v>
@@ -4388,7 +4382,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="U8" s="3" t="e" vm="65">
         <v>#VALUE!</v>
@@ -4407,10 +4401,10 @@
       <c r="B9" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="8" t="e" vm="67">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D9" s="9"/>
+      <c r="C9" s="5" t="e" vm="67">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D9" s="3"/>
       <c r="E9" s="3" t="e" vm="68">
         <v>#VALUE!</v>
       </c>
@@ -4423,13 +4417,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K9" s="3" t="e" vm="71">
         <v>#VALUE!</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M9" s="3" t="e" vm="72">
         <v>#VALUE!</v>
@@ -4447,7 +4441,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="U9" s="3" t="e" vm="76">
         <v>#VALUE!</v>
@@ -4464,19 +4458,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C10" s="8" t="e" vm="78">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>186</v>
+        <v>180</v>
+      </c>
+      <c r="C10" s="5" t="e" vm="78">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="E10" s="3" t="e" vm="79">
         <v>#VALUE!</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G10" s="3" t="e" vm="80">
         <v>#VALUE!</v>
@@ -4485,7 +4479,9 @@
       <c r="I10" s="3" t="e" vm="81">
         <v>#VALUE!</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="K10" s="3" t="e" vm="82">
         <v>#VALUE!</v>
       </c>
@@ -4494,19 +4490,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O10" s="3" t="e" vm="84">
         <v>#VALUE!</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="Q10" s="3" t="e" vm="85">
         <v>#VALUE!</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="S10" s="3" t="e" vm="86">
         <v>#VALUE!</v>
@@ -4520,7 +4516,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Y10" s="3"/>
     </row>
@@ -4529,12 +4525,12 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="8" t="e" vm="89">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D11" s="9"/>
+        <v>173</v>
+      </c>
+      <c r="C11" s="5" t="e" vm="89">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D11" s="3"/>
       <c r="E11" s="3" t="e" vm="90">
         <v>#VALUE!</v>
       </c>
@@ -4552,19 +4548,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="M11" s="3" t="e" vm="94">
         <v>#VALUE!</v>
       </c>
       <c r="N11" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="O11" s="3" t="e" vm="95">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P11" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="O11" s="3" t="e" vm="95">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="Q11" s="3" t="e" vm="96">
         <v>#VALUE!</v>
@@ -4574,7 +4570,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="U11" s="3" t="e" vm="98">
         <v>#VALUE!</v>
@@ -4584,7 +4580,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Y11" s="3"/>
     </row>
@@ -4595,11 +4591,11 @@
       <c r="B12" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="8" t="e" vm="100">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>135</v>
+      <c r="C12" s="5" t="e" vm="100">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="E12" s="3" t="e" vm="101">
         <v>#VALUE!</v>
@@ -4629,25 +4625,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="S12" s="3" t="e" vm="108">
         <v>#VALUE!</v>
       </c>
       <c r="T12" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="U12" s="3" t="e" vm="109">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="W12" s="3" t="e" vm="110">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X12" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="U12" s="3" t="e" vm="109">
-        <v>#VALUE!</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="W12" s="3" t="e" vm="110">
-        <v>#VALUE!</v>
-      </c>
-      <c r="X12" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="Y12" s="3"/>
     </row>
@@ -4658,17 +4654,17 @@
       <c r="B13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="8" t="e" vm="111">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>150</v>
+      <c r="C13" s="5" t="e" vm="111">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="E13" s="3" t="e" vm="112">
         <v>#VALUE!</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G13" s="3" t="e" vm="113">
         <v>#VALUE!</v>
@@ -4680,49 +4676,49 @@
         <v>#VALUE!</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K13" s="3" t="e" vm="115">
         <v>#VALUE!</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M13" s="3" t="e" vm="116">
         <v>#VALUE!</v>
       </c>
       <c r="N13" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="O13" s="3" t="e" vm="117">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q13" s="3" t="e" vm="118">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="S13" s="3" t="e" vm="119">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="U13" s="3" t="e" vm="120">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V13" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="O13" s="3" t="e" vm="117">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q13" s="3" t="e" vm="118">
-        <v>#VALUE!</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="S13" s="3" t="e" vm="119">
-        <v>#VALUE!</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="U13" s="3" t="e" vm="120">
-        <v>#VALUE!</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="W13" s="3" t="e" vm="121">
         <v>#VALUE!</v>
       </c>
       <c r="X13" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y13" s="3"/>
     </row>
@@ -4733,10 +4729,10 @@
       <c r="B14" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="8" t="e" vm="122">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D14" s="9"/>
+      <c r="C14" s="5" t="e" vm="122">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D14" s="3"/>
       <c r="E14" s="3" t="e" vm="123">
         <v>#VALUE!</v>
       </c>
@@ -4745,7 +4741,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I14" s="3" t="e" vm="125">
         <v>#VALUE!</v>
@@ -4763,19 +4759,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="Q14" s="3" t="e" vm="129">
         <v>#VALUE!</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="S14" s="3" t="e" vm="130">
         <v>#VALUE!</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="U14" s="3" t="e" vm="131">
         <v>#VALUE!</v>
@@ -4949,9 +4945,6 @@
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -4977,9 +4970,6 @@
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -5053,9 +5043,6 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -5079,9 +5066,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -5102,15 +5087,10 @@
       <c r="W26" s="2"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -5134,17 +5114,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="U1:V1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial commit for 3.24 Necropolis league
</commit_message>
<xml_diff>
--- a/Scraps.xlsx
+++ b/Scraps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E257C0-EB57-45FA-B9FC-1A456566C57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CFB7C0-22C2-41BC-A975-B2A0A4FD1322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
+    <workbookView xWindow="9225" yWindow="2640" windowWidth="27060" windowHeight="14805" activeTab="1" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Icons" sheetId="1" r:id="rId1"/>
@@ -1367,7 +1367,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="199">
   <si>
     <t>Circle</t>
   </si>
@@ -1828,18 +1828,6 @@
     <t>Scarab</t>
   </si>
   <si>
-    <t>Winged</t>
-  </si>
-  <si>
-    <t>Gilded</t>
-  </si>
-  <si>
-    <t>Rusted</t>
-  </si>
-  <si>
-    <t>Polished</t>
-  </si>
-  <si>
     <t>Uber Elder</t>
   </si>
   <si>
@@ -1861,9 +1849,6 @@
     <t>Level 21/23 Qual</t>
   </si>
   <si>
-    <t>Maven's Invitation</t>
-  </si>
-  <si>
     <t>Atlas Invitation</t>
   </si>
   <si>
@@ -1903,9 +1888,6 @@
     <t>Elderslayer</t>
   </si>
   <si>
-    <t>Affliction Charms/Tinctures</t>
-  </si>
-  <si>
     <t>Cluster Jewels</t>
   </si>
   <si>
@@ -1967,6 +1949,21 @@
   </si>
   <si>
     <t>Unique</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Rare?</t>
+  </si>
+  <si>
+    <t>Scarab of</t>
+  </si>
+  <si>
+    <t>Coffins/Embers</t>
+  </si>
+  <si>
+    <t>Tattoos</t>
   </si>
 </sst>
 </file>
@@ -2031,7 +2028,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2041,9 +2038,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2861,9 +2855,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2901,7 +2895,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3007,7 +3001,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3149,7 +3143,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3874,8 +3868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EF3207-198A-49F7-97F5-E86C821AC6FF}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3909,56 +3903,56 @@
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8" t="s">
+      <c r="N1" s="7"/>
+      <c r="O1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8" t="s">
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8" t="s">
+      <c r="R1" s="7"/>
+      <c r="S1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8" t="s">
+      <c r="T1" s="7"/>
+      <c r="U1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8" t="s">
+      <c r="V1" s="7"/>
+      <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="8"/>
+      <c r="X1" s="7"/>
       <c r="Y1" s="3"/>
     </row>
     <row r="2" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="5"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -3987,77 +3981,77 @@
       <c r="Y2" s="3"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="7" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="6" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E3" s="6" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="5" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="6" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="I3" s="6" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="K3" s="6" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="M3" s="6" t="e" vm="6">
-        <v>#VALUE!</v>
-      </c>
-      <c r="N3" s="6" t="s">
+      <c r="G3" s="5" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="I3" s="5" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="K3" s="5" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="M3" s="5" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="O3" s="6" t="e" vm="7">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P3" s="6" t="s">
+      <c r="O3" s="5" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Q3" s="6" t="e" vm="8">
-        <v>#VALUE!</v>
-      </c>
-      <c r="R3" s="6" t="s">
+      <c r="Q3" s="5" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="S3" s="6" t="e" vm="9">
-        <v>#VALUE!</v>
-      </c>
-      <c r="T3" s="6" t="s">
+      <c r="S3" s="5" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T3" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="U3" s="6" t="e" vm="10">
-        <v>#VALUE!</v>
-      </c>
-      <c r="V3" s="6" t="s">
+      <c r="U3" s="5" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V3" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="W3" s="6" t="e" vm="11">
-        <v>#VALUE!</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>191</v>
+      <c r="W3" s="5" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="Y3" s="3"/>
     </row>
@@ -4068,7 +4062,7 @@
       <c r="B4" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="5" t="e" vm="12">
+      <c r="C4" s="4" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="D4" s="3"/>
@@ -4079,6 +4073,7 @@
       <c r="G4" s="3" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
+      <c r="H4" s="2"/>
       <c r="I4" s="3" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
@@ -4087,19 +4082,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="M4" s="3" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>156</v>
+        <v>196</v>
       </c>
       <c r="O4" s="3" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>154</v>
+        <v>47</v>
       </c>
       <c r="Q4" s="3" t="e" vm="19">
         <v>#VALUE!</v>
@@ -4109,7 +4104,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="U4" s="3" t="e" vm="21">
         <v>#VALUE!</v>
@@ -4126,9 +4121,9 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5" s="5" t="e" vm="23">
+        <v>164</v>
+      </c>
+      <c r="C5" s="4" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -4138,18 +4133,20 @@
         <v>#VALUE!</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G5" s="3" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I5" s="3" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="K5" s="3" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
@@ -4179,13 +4176,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="W5" s="3" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="Y5" s="3"/>
     </row>
@@ -4196,7 +4193,7 @@
       <c r="B6" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="5" t="e" vm="34">
+      <c r="C6" s="4" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -4236,7 +4233,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="Q6" s="3" t="e" vm="41">
         <v>#VALUE!</v>
@@ -4269,13 +4266,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C7" s="5" t="e" vm="45">
+        <v>156</v>
+      </c>
+      <c r="C7" s="4" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E7" s="3" t="e" vm="46">
         <v>#VALUE!</v>
@@ -4289,7 +4286,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K7" s="3" t="e" vm="49">
         <v>#VALUE!</v>
@@ -4299,25 +4296,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="O7" s="3" t="e" vm="51">
         <v>#VALUE!</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="Q7" s="3" t="e" vm="52">
         <v>#VALUE!</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="S7" s="3" t="e" vm="53">
         <v>#VALUE!</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="U7" s="3" t="e" vm="54">
         <v>#VALUE!</v>
@@ -4334,13 +4331,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C8" s="5" t="e" vm="56">
+        <v>180</v>
+      </c>
+      <c r="C8" s="4" t="e" vm="56">
         <v>#VALUE!</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E8" s="3" t="e" vm="57">
         <v>#VALUE!</v>
@@ -4350,7 +4347,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="I8" s="3" t="e" vm="59">
         <v>#VALUE!</v>
@@ -4360,7 +4357,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="M8" s="3" t="e" vm="61">
         <v>#VALUE!</v>
@@ -4372,7 +4369,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="Q8" s="3" t="e" vm="63">
         <v>#VALUE!</v>
@@ -4382,7 +4379,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="U8" s="3" t="e" vm="65">
         <v>#VALUE!</v>
@@ -4398,10 +4395,10 @@
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="5" t="e" vm="67">
+      <c r="C9" s="4" t="e" vm="67">
         <v>#VALUE!</v>
       </c>
       <c r="D9" s="3"/>
@@ -4412,23 +4409,23 @@
       <c r="G9" s="3" t="e" vm="69">
         <v>#VALUE!</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="2"/>
       <c r="I9" s="3" t="e" vm="70">
         <v>#VALUE!</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K9" s="3" t="e" vm="71">
         <v>#VALUE!</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>197</v>
+      <c r="L9" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="M9" s="3" t="e" vm="72">
         <v>#VALUE!</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="2"/>
       <c r="O9" s="3" t="e" vm="73">
         <v>#VALUE!</v>
       </c>
@@ -4440,7 +4437,7 @@
       <c r="S9" s="3" t="e" vm="75">
         <v>#VALUE!</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="T9" s="2" t="s">
         <v>142</v>
       </c>
       <c r="U9" s="3" t="e" vm="76">
@@ -4458,19 +4455,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="5" t="e" vm="78">
+        <v>174</v>
+      </c>
+      <c r="C10" s="4" t="e" vm="78">
         <v>#VALUE!</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E10" s="3" t="e" vm="79">
         <v>#VALUE!</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G10" s="3" t="e" vm="80">
         <v>#VALUE!</v>
@@ -4480,7 +4477,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="K10" s="3" t="e" vm="82">
         <v>#VALUE!</v>
@@ -4490,13 +4487,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="O10" s="3" t="e" vm="84">
         <v>#VALUE!</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="Q10" s="3" t="e" vm="85">
         <v>#VALUE!</v>
@@ -4525,9 +4522,9 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C11" s="5" t="e" vm="89">
+        <v>168</v>
+      </c>
+      <c r="C11" s="4" t="e" vm="89">
         <v>#VALUE!</v>
       </c>
       <c r="D11" s="3"/>
@@ -4544,11 +4541,12 @@
       <c r="I11" s="3" t="e" vm="92">
         <v>#VALUE!</v>
       </c>
+      <c r="J11" s="2"/>
       <c r="K11" s="3" t="e" vm="93">
         <v>#VALUE!</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="M11" s="3" t="e" vm="94">
         <v>#VALUE!</v>
@@ -4570,7 +4568,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="U11" s="3" t="e" vm="98">
         <v>#VALUE!</v>
@@ -4591,7 +4589,7 @@
       <c r="B12" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="5" t="e" vm="100">
+      <c r="C12" s="4" t="e" vm="100">
         <v>#VALUE!</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -4654,7 +4652,7 @@
       <c r="B13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="5" t="e" vm="111">
+      <c r="C13" s="4" t="e" vm="111">
         <v>#VALUE!</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -4676,49 +4674,47 @@
         <v>#VALUE!</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="K13" s="3" t="e" vm="115">
         <v>#VALUE!</v>
       </c>
       <c r="L13" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="M13" s="3" t="e" vm="116">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O13" s="3" t="e" vm="117">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q13" s="3" t="e" vm="118">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R13" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="M13" s="3" t="e" vm="116">
-        <v>#VALUE!</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="O13" s="3" t="e" vm="117">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q13" s="3" t="e" vm="118">
-        <v>#VALUE!</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="S13" s="3" t="e" vm="119">
         <v>#VALUE!</v>
       </c>
-      <c r="T13" s="3" t="s">
-        <v>164</v>
-      </c>
+      <c r="T13" s="3"/>
       <c r="U13" s="3" t="e" vm="120">
         <v>#VALUE!</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="W13" s="3" t="e" vm="121">
         <v>#VALUE!</v>
       </c>
       <c r="X13" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="Y13" s="3"/>
     </row>
@@ -4729,7 +4725,7 @@
       <c r="B14" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="5" t="e" vm="122">
+      <c r="C14" s="4" t="e" vm="122">
         <v>#VALUE!</v>
       </c>
       <c r="D14" s="3"/>
@@ -4764,8 +4760,8 @@
       <c r="Q14" s="3" t="e" vm="129">
         <v>#VALUE!</v>
       </c>
-      <c r="R14" s="1" t="s">
-        <v>195</v>
+      <c r="R14" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="S14" s="3" t="e" vm="130">
         <v>#VALUE!</v>
@@ -5114,17 +5110,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="U1:V1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="U1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First week of Necropolis changes
</commit_message>
<xml_diff>
--- a/Scraps.xlsx
+++ b/Scraps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CFB7C0-22C2-41BC-A975-B2A0A4FD1322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD34E81-FEDA-4BCF-BE32-F84C6DFBD974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9225" yWindow="2640" windowWidth="27060" windowHeight="14805" activeTab="1" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
+    <workbookView xWindow="1755" yWindow="2640" windowWidth="34530" windowHeight="15120" activeTab="1" xr2:uid="{C288C689-496E-4B6C-81C5-101C6A0A59F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Icons" sheetId="1" r:id="rId1"/>
@@ -1367,7 +1367,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="198">
   <si>
     <t>Circle</t>
   </si>
@@ -1784,9 +1784,6 @@
   </si>
   <si>
     <t>Vaal Orb</t>
-  </si>
-  <si>
-    <t>Sextant</t>
   </si>
   <si>
     <t>Eldritch</t>
@@ -3868,8 +3865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EF3207-198A-49F7-97F5-E86C821AC6FF}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3997,25 +3994,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G3" s="5" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I3" s="5" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="K3" s="5" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="K3" s="5" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="M3" s="5" t="e" vm="6">
         <v>#VALUE!</v>
@@ -4027,14 +4024,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q3" s="5" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
-      <c r="R3" s="5" t="s">
-        <v>139</v>
-      </c>
+      <c r="R3" s="5"/>
       <c r="S3" s="5" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
@@ -4051,7 +4046,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Y3" s="3"/>
     </row>
@@ -4060,7 +4055,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="4" t="e" vm="12">
         <v>#VALUE!</v>
@@ -4082,13 +4077,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M4" s="3" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O4" s="3" t="e" vm="18">
         <v>#VALUE!</v>
@@ -4104,7 +4099,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U4" s="3" t="e" vm="21">
         <v>#VALUE!</v>
@@ -4121,7 +4116,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" s="4" t="e" vm="23">
         <v>#VALUE!</v>
@@ -4133,19 +4128,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G5" s="3" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I5" s="3" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K5" s="3" t="e" vm="27">
         <v>#VALUE!</v>
@@ -4176,13 +4171,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="W5" s="3" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Y5" s="3"/>
     </row>
@@ -4233,7 +4228,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q6" s="3" t="e" vm="41">
         <v>#VALUE!</v>
@@ -4266,13 +4261,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C7" s="4" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E7" s="3" t="e" vm="46">
         <v>#VALUE!</v>
@@ -4286,7 +4281,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K7" s="3" t="e" vm="49">
         <v>#VALUE!</v>
@@ -4296,25 +4291,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O7" s="3" t="e" vm="51">
         <v>#VALUE!</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q7" s="3" t="e" vm="52">
         <v>#VALUE!</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S7" s="3" t="e" vm="53">
         <v>#VALUE!</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U7" s="3" t="e" vm="54">
         <v>#VALUE!</v>
@@ -4331,13 +4326,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C8" s="4" t="e" vm="56">
         <v>#VALUE!</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E8" s="3" t="e" vm="57">
         <v>#VALUE!</v>
@@ -4347,7 +4342,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I8" s="3" t="e" vm="59">
         <v>#VALUE!</v>
@@ -4357,7 +4352,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M8" s="3" t="e" vm="61">
         <v>#VALUE!</v>
@@ -4369,7 +4364,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q8" s="3" t="e" vm="63">
         <v>#VALUE!</v>
@@ -4379,7 +4374,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U8" s="3" t="e" vm="65">
         <v>#VALUE!</v>
@@ -4414,13 +4409,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K9" s="3" t="e" vm="71">
         <v>#VALUE!</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M9" s="3" t="e" vm="72">
         <v>#VALUE!</v>
@@ -4438,7 +4433,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="U9" s="3" t="e" vm="76">
         <v>#VALUE!</v>
@@ -4455,19 +4450,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" s="4" t="e" vm="78">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="3" t="e" vm="79">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C10" s="4" t="e" vm="78">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E10" s="3" t="e" vm="79">
-        <v>#VALUE!</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="G10" s="3" t="e" vm="80">
         <v>#VALUE!</v>
@@ -4477,7 +4472,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K10" s="3" t="e" vm="82">
         <v>#VALUE!</v>
@@ -4487,19 +4482,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O10" s="3" t="e" vm="84">
         <v>#VALUE!</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q10" s="3" t="e" vm="85">
         <v>#VALUE!</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S10" s="3" t="e" vm="86">
         <v>#VALUE!</v>
@@ -4513,7 +4508,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y10" s="3"/>
     </row>
@@ -4522,7 +4517,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C11" s="4" t="e" vm="89">
         <v>#VALUE!</v>
@@ -4546,19 +4541,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M11" s="3" t="e" vm="94">
         <v>#VALUE!</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O11" s="3" t="e" vm="95">
         <v>#VALUE!</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Q11" s="3" t="e" vm="96">
         <v>#VALUE!</v>
@@ -4568,7 +4563,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U11" s="3" t="e" vm="98">
         <v>#VALUE!</v>
@@ -4578,7 +4573,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Y11" s="3"/>
     </row>
@@ -4656,13 +4651,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="3" t="e" vm="112">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="E13" s="3" t="e" vm="112">
-        <v>#VALUE!</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="G13" s="3" t="e" vm="113">
         <v>#VALUE!</v>
@@ -4674,31 +4669,31 @@
         <v>#VALUE!</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K13" s="3" t="e" vm="115">
         <v>#VALUE!</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M13" s="3" t="e" vm="116">
         <v>#VALUE!</v>
       </c>
       <c r="N13" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="O13" s="3" t="e" vm="117">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P13" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="O13" s="3" t="e" vm="117">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="Q13" s="3" t="e" vm="118">
         <v>#VALUE!</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S13" s="3" t="e" vm="119">
         <v>#VALUE!</v>
@@ -4708,13 +4703,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="W13" s="3" t="e" vm="121">
         <v>#VALUE!</v>
       </c>
       <c r="X13" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Y13" s="3"/>
     </row>
@@ -4737,7 +4732,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I14" s="3" t="e" vm="125">
         <v>#VALUE!</v>
@@ -4755,19 +4750,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q14" s="3" t="e" vm="129">
         <v>#VALUE!</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="S14" s="3" t="e" vm="130">
         <v>#VALUE!</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="U14" s="3" t="e" vm="131">
         <v>#VALUE!</v>
@@ -5110,17 +5105,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="U1:V1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="U1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>